<commit_message>
Update README.md and imgs
</commit_message>
<xml_diff>
--- a/01-Prevendo-valores-no-Excel/Apartamentos_Relatorio.xlsx
+++ b/01-Prevendo-valores-no-Excel/Apartamentos_Relatorio.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Apartamentos - Simples" sheetId="1" r:id="rId1"/>
@@ -337,9 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -348,6 +345,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3201,7 +3201,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="437" row="2">
+  <wetp:taskpane dockstate="right" visibility="1" width="437" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -3214,7 +3214,7 @@
     <we:reference id="wa104379638" version="1.0.0.0" store="wa104379638" storeType="OMEX"/>
   </we:alternateReferences>
   <we:properties>
-    <we:property name="endpoints" value="&quot;[{\&quot;documentationUrl\&quot;:\&quot;https://ussouthcentral.services.azureml.net/workspaces/52a9fe1f0655445a9ec08cbaf87c3ffa/services/2a951e49ed8d43cfbe3afc68aa6d3878/swagger.json\&quot;,\&quot;token\&quot;:\&quot;xSc38GPprrK3FGyGMn5uQEJVD7wNUZgOn2UZt+vrFLMLFAyqGB+YhkF5o0JH57hfUYuIxZ7so1rf5DQ2nDfdGA==\&quot;,\&quot;serviceName\&quot;:\&quot;Titanic Survivor Predictor (Excel Add-in Sample) [Score]\&quot;,\&quot;globalParametersValues\&quot;:{},\&quot;outputCellValues\&quot;:{},\&quot;showOverwriteWarning\&quot;:true},{\&quot;documentationUrl\&quot;:\&quot;https://ussouthcentral.services.azureml.net/odata/workspaces/52a9fe1f0655445a9ec08cbaf87c3ffa/services/0153ed4ecce44d999e7846d8f0e8102a\&quot;,\&quot;token\&quot;:\&quot;QR+dXhrglxsnO5WJ4/s0me85cwO+4WF7FcWVoUUSqFwzGyFCYbMIpzYfSaMwkNdNJGGavTDvVTlNbP1gv9Yh9A==\&quot;,\&quot;serviceName\&quot;:\&quot;Text Sentiment Analysis (Excel Add-in Sample) [Score]\&quot;,\&quot;globalParametersValues\&quot;:{},\&quot;outputCellValues\&quot;:{},\&quot;showOverwriteWarning\&quot;:true},{\&quot;documentationUrl\&quot;:\&quot;https://studio.azureml.net/apihelp/workspaces/66940729eee34b3cbd0ad7a8d166cc3f/webservices/c5d10e63c30c40bcae122464973ec333/endpoints/e5b092e76c644f9c9be869bb5f8e266e/score\&quot;,\&quot;token\&quot;:\&quot;NkQd11NEi0lW2ctR04DnUQTv8yY0zlQPzKAM6rP3z8motDqwuQaranX67yyJ3RjCB7HNpMPlTeZXLsr2RtGwPw==\&quot;,\&quot;serviceName\&quot;:\&quot;Apartamentos 01 [Predictive Exp.]\&quot;,\&quot;globalParametersValues\&quot;:{},\&quot;outputCellValues\&quot;:{\&quot;output1\&quot;:{\&quot;id\&quot;:\&quot;'Apartamentos - Multipla'!K6\&quot;,\&quot;includeHeaders\&quot;:false}},\&quot;showOverwriteWarning\&quot;:true,\&quot;inputBindingsAddresses\&quot;:{\&quot;input1\&quot;:{\&quot;bindingAddress\&quot;:\&quot;'Apartamentos - Multipla'!G6:J9\&quot;,\&quot;hasHeaders\&quot;:false}}}]&quot;"/>
+    <we:property name="endpoints" value="&quot;[{\&quot;documentationUrl\&quot;:\&quot;https://ussouthcentral.services.azureml.net/workspaces/52a9fe1f0655445a9ec08cbaf87c3ffa/services/2a951e49ed8d43cfbe3afc68aa6d3878/swagger.json\&quot;,\&quot;token\&quot;:\&quot;xSc38GPprrK3FGyGMn5uQEJVD7wNUZgOn2UZt+vrFLMLFAyqGB+YhkF5o0JH57hfUYuIxZ7so1rf5DQ2nDfdGA==\&quot;,\&quot;serviceName\&quot;:\&quot;Titanic Survivor Predictor (Excel Add-in Sample) [Score]\&quot;,\&quot;globalParametersValues\&quot;:{},\&quot;outputCellValues\&quot;:{},\&quot;showOverwriteWarning\&quot;:true},{\&quot;documentationUrl\&quot;:\&quot;https://ussouthcentral.services.azureml.net/odata/workspaces/52a9fe1f0655445a9ec08cbaf87c3ffa/services/0153ed4ecce44d999e7846d8f0e8102a\&quot;,\&quot;token\&quot;:\&quot;QR+dXhrglxsnO5WJ4/s0me85cwO+4WF7FcWVoUUSqFwzGyFCYbMIpzYfSaMwkNdNJGGavTDvVTlNbP1gv9Yh9A==\&quot;,\&quot;serviceName\&quot;:\&quot;Text Sentiment Analysis (Excel Add-in Sample) [Score]\&quot;,\&quot;globalParametersValues\&quot;:{},\&quot;outputCellValues\&quot;:{},\&quot;showOverwriteWarning\&quot;:true}]&quot;"/>
   </we:properties>
   <we:bindings>
     <we:binding id="UnnamedBinding_0_1461262394414" type="matrix" appref="{9067955A-BAD9-4D8D-86D8-8DE530DCD771}"/>
@@ -3222,6 +3222,10 @@
     <we:binding id="UnnamedBinding_2_1461262405260" type="matrix" appref="{EB2E7B5D-FE72-4836-B572-BCDA994FF728}"/>
     <we:binding id="'Apartamentos - Multipla'!K6:K9" type="matrix" appref="{8CFA8034-8D8C-4072-B955-31F946190A58}"/>
     <we:binding id="UnnamedBinding_3_1461262498496" type="matrix" appref="{D0F3CB8E-A8B5-4853-A2DD-1B3AD5E37B2A}"/>
+    <we:binding id="UnnamedBinding_0_1461266951927" type="matrix" appref="{19CBA43A-E8DC-4DA5-8C27-C54FD95183CF}"/>
+    <we:binding id="UnnamedBinding_1_1461266999739" type="matrix" appref="{42B04561-6A0D-4A66-969E-F05BC3638ECB}"/>
+    <we:binding id="UnnamedBinding_2_1461266999762" type="matrix" appref="{54B6D913-A905-485B-9F0F-5BE8B8032681}"/>
+    <we:binding id="UnnamedBinding_3_1461266999837" type="matrix" appref="{EE5F4B49-9D24-482D-B5CB-A00F33F5F7E7}"/>
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
@@ -3256,10 +3260,10 @@
       <c r="B2" s="1">
         <v>890</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -3577,9 +3581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3659,7 +3661,7 @@
       <c r="E4" s="1">
         <v>1188</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3679,19 +3681,19 @@
       <c r="E5" s="1">
         <v>890</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3723,7 +3725,7 @@
       <c r="J6">
         <v>35</v>
       </c>
-      <c r="K6" s="15"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -3753,7 +3755,7 @@
       <c r="J7">
         <v>85</v>
       </c>
-      <c r="K7" s="15"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -3783,7 +3785,7 @@
       <c r="J8">
         <v>150</v>
       </c>
-      <c r="K8" s="15"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -3813,7 +3815,7 @@
       <c r="J9">
         <v>60</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -4248,6 +4250,18 @@
         <x15:webExtension appRef="{D0F3CB8E-A8B5-4853-A2DD-1B3AD5E37B2A}">
           <xm:f>'Apartamentos - Multipla'!$G$6:$J$9</xm:f>
         </x15:webExtension>
+        <x15:webExtension appRef="{19CBA43A-E8DC-4DA5-8C27-C54FD95183CF}">
+          <xm:f>'Apartamentos - Multipla'!$G$6:$J$9</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{42B04561-6A0D-4A66-969E-F05BC3638ECB}">
+          <xm:f>'Apartamentos - Multipla'!K6</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{54B6D913-A905-485B-9F0F-5BE8B8032681}">
+          <xm:f>'Apartamentos - Multipla'!K6</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{EE5F4B49-9D24-482D-B5CB-A00F33F5F7E7}">
+          <xm:f>'Apartamentos - Multipla'!$G$6:$J$9</xm:f>
+        </x15:webExtension>
       </x15:webExtensions>
     </ext>
   </extLst>
@@ -4258,7 +4272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>